<commit_message>
linter, stat skeleton, start commenting
</commit_message>
<xml_diff>
--- a/avgs by season.xlsx
+++ b/avgs by season.xlsx
@@ -959,11 +959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-724197680"/>
-        <c:axId val="-723613264"/>
+        <c:axId val="1071461872"/>
+        <c:axId val="1045885568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-724197680"/>
+        <c:axId val="1071461872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -1022,12 +1022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-723613264"/>
+        <c:crossAx val="1045885568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-723613264"/>
+        <c:axId val="1045885568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="88.0"/>
@@ -1085,7 +1085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-724197680"/>
+        <c:crossAx val="1071461872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1515,11 +1515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-723626912"/>
-        <c:axId val="-778824048"/>
+        <c:axId val="1090822176"/>
+        <c:axId val="1090824496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-723626912"/>
+        <c:axId val="1090822176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34.0"/>
@@ -1578,12 +1578,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-778824048"/>
+        <c:crossAx val="1090824496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-778824048"/>
+        <c:axId val="1090824496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-723626912"/>
+        <c:crossAx val="1090822176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,6 +1711,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1744,6 +1747,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2226,11 +2232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-700019952"/>
-        <c:axId val="-700193760"/>
+        <c:axId val="1044557088"/>
+        <c:axId val="1044599376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-700019952"/>
+        <c:axId val="1044557088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2275,6 +2281,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2289,12 +2298,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700193760"/>
+        <c:crossAx val="1044599376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-700193760"/>
+        <c:axId val="1044599376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.56"/>
@@ -2339,6 +2348,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2353,7 +2365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700019952"/>
+        <c:crossAx val="1044557088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2389,7 +2401,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2940,11 +2956,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-699902736"/>
-        <c:axId val="-699900688"/>
+        <c:axId val="1071307328"/>
+        <c:axId val="1071300496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-699902736"/>
+        <c:axId val="1071307328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -3003,12 +3019,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-699900688"/>
+        <c:crossAx val="1071300496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-699900688"/>
+        <c:axId val="1071300496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75.0"/>
@@ -3067,7 +3083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-699902736"/>
+        <c:crossAx val="1071307328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3484,11 +3500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-700339904"/>
-        <c:axId val="-700392080"/>
+        <c:axId val="1090742880"/>
+        <c:axId val="1090556880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-700339904"/>
+        <c:axId val="1090742880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="118.0"/>
@@ -3546,12 +3562,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700392080"/>
+        <c:crossAx val="1090556880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-700392080"/>
+        <c:axId val="1090556880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.24"/>
@@ -3609,7 +3625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700339904"/>
+        <c:crossAx val="1090742880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4196,11 +4212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-772948912"/>
-        <c:axId val="-772946864"/>
+        <c:axId val="1090685104"/>
+        <c:axId val="1090687152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-772948912"/>
+        <c:axId val="1090685104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -4258,12 +4274,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-772946864"/>
+        <c:crossAx val="1090687152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-772946864"/>
+        <c:axId val="1090687152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="85.0"/>
@@ -4320,7 +4336,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-772948912"/>
+        <c:crossAx val="1090685104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4769,11 +4785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-773181344"/>
-        <c:axId val="-773179296"/>
+        <c:axId val="1090797344"/>
+        <c:axId val="1090798976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-773181344"/>
+        <c:axId val="1090797344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -4832,12 +4848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773179296"/>
+        <c:crossAx val="1090798976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-773179296"/>
+        <c:axId val="1090798976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34.0"/>
@@ -4896,7 +4912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773181344"/>
+        <c:crossAx val="1090797344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5483,11 +5499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-700374496"/>
-        <c:axId val="-700372448"/>
+        <c:axId val="1071438128"/>
+        <c:axId val="1071440176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-700374496"/>
+        <c:axId val="1071438128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -5545,12 +5561,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700372448"/>
+        <c:crossAx val="1071440176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-700372448"/>
+        <c:axId val="1071440176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.35"/>
@@ -5608,7 +5624,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-700374496"/>
+        <c:crossAx val="1071438128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6056,11 +6072,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-772873888"/>
-        <c:axId val="-772870320"/>
+        <c:axId val="1072391616"/>
+        <c:axId val="1072010992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-772873888"/>
+        <c:axId val="1072391616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -6082,6 +6098,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6118,12 +6135,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-772870320"/>
+        <c:crossAx val="1072010992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-772870320"/>
+        <c:axId val="1072010992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
@@ -6182,7 +6199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-772873888"/>
+        <c:crossAx val="1072391616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6505,11 +6522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-723677520"/>
-        <c:axId val="-723675744"/>
+        <c:axId val="1071622448"/>
+        <c:axId val="1071624496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-723677520"/>
+        <c:axId val="1071622448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6566,12 +6583,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-723675744"/>
+        <c:crossAx val="1071624496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-723675744"/>
+        <c:axId val="1071624496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6627,7 +6644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-723677520"/>
+        <c:crossAx val="1071622448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14248,8 +14265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF77" sqref="AF77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
generally working, but super old seasons have bad data - bob schafer doesn't have an age - so fix empty col bug asap, though works 100% for correct data
</commit_message>
<xml_diff>
--- a/avgs by season.xlsx
+++ b/avgs by season.xlsx
@@ -959,11 +959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163541440"/>
-        <c:axId val="1163519600"/>
+        <c:axId val="1161167584"/>
+        <c:axId val="1161169632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163541440"/>
+        <c:axId val="1161167584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -1022,12 +1022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163519600"/>
+        <c:crossAx val="1161169632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163519600"/>
+        <c:axId val="1161169632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="88.0"/>
@@ -1085,7 +1085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163541440"/>
+        <c:crossAx val="1161167584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1178,6 +1178,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1514,11 +1515,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163293168"/>
-        <c:axId val="1163295488"/>
+        <c:axId val="1158083952"/>
+        <c:axId val="1158086272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163293168"/>
+        <c:axId val="1158083952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34.0"/>
@@ -1577,12 +1578,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163295488"/>
+        <c:crossAx val="1158086272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163295488"/>
+        <c:axId val="1158086272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,7 +1639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163293168"/>
+        <c:crossAx val="1158083952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1728,6 +1729,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2050,11 +2052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1155239472"/>
-        <c:axId val="1155241648"/>
+        <c:axId val="1158098944"/>
+        <c:axId val="1158100992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1155239472"/>
+        <c:axId val="1158098944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="118.0"/>
@@ -2112,12 +2114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1155241648"/>
+        <c:crossAx val="1158100992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1155241648"/>
+        <c:axId val="1158100992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.35"/>
@@ -2174,7 +2176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1155239472"/>
+        <c:crossAx val="1158098944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2766,11 +2768,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163533376"/>
-        <c:axId val="1163535424"/>
+        <c:axId val="1161122032"/>
+        <c:axId val="1161148432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163533376"/>
+        <c:axId val="1161122032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2832,12 +2834,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163535424"/>
+        <c:crossAx val="1161148432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163535424"/>
+        <c:axId val="1161148432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.56"/>
@@ -2899,7 +2901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163533376"/>
+        <c:crossAx val="1161122032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3490,11 +3492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163471872"/>
-        <c:axId val="1163473920"/>
+        <c:axId val="1161046352"/>
+        <c:axId val="1161040320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163471872"/>
+        <c:axId val="1161046352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -3553,12 +3555,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163473920"/>
+        <c:crossAx val="1161040320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163473920"/>
+        <c:axId val="1161040320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="75.0"/>
@@ -3617,7 +3619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163471872"/>
+        <c:crossAx val="1161046352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4034,11 +4036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163468496"/>
-        <c:axId val="1163445408"/>
+        <c:axId val="1160976528"/>
+        <c:axId val="1160978576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163468496"/>
+        <c:axId val="1160976528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="118.0"/>
@@ -4097,12 +4099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163445408"/>
+        <c:crossAx val="1160978576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163445408"/>
+        <c:axId val="1160978576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.24"/>
@@ -4160,7 +4162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163468496"/>
+        <c:crossAx val="1160976528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4747,11 +4749,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163412208"/>
-        <c:axId val="1163414256"/>
+        <c:axId val="1158184784"/>
+        <c:axId val="1065758304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163412208"/>
+        <c:axId val="1158184784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -4810,12 +4812,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163414256"/>
+        <c:crossAx val="1065758304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163414256"/>
+        <c:axId val="1065758304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="85.0"/>
@@ -4872,7 +4874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163412208"/>
+        <c:crossAx val="1158184784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5321,11 +5323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163409168"/>
-        <c:axId val="1163396736"/>
+        <c:axId val="1160835808"/>
+        <c:axId val="1160837856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163409168"/>
+        <c:axId val="1160835808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -5384,12 +5386,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163396736"/>
+        <c:crossAx val="1160837856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163396736"/>
+        <c:axId val="1160837856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34.0"/>
@@ -5448,7 +5450,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163409168"/>
+        <c:crossAx val="1160835808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6035,11 +6037,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163359840"/>
-        <c:axId val="1163361888"/>
+        <c:axId val="1158141216"/>
+        <c:axId val="1158143264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163359840"/>
+        <c:axId val="1158141216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -6097,12 +6099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163361888"/>
+        <c:crossAx val="1158143264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163361888"/>
+        <c:axId val="1158143264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.35"/>
@@ -6160,7 +6162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163359840"/>
+        <c:crossAx val="1158141216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6608,11 +6610,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1163321824"/>
-        <c:axId val="1163323872"/>
+        <c:axId val="1162743616"/>
+        <c:axId val="1158152704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1163321824"/>
+        <c:axId val="1162743616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -6671,12 +6673,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163323872"/>
+        <c:crossAx val="1158152704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1163323872"/>
+        <c:axId val="1158152704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
@@ -6735,7 +6737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1163321824"/>
+        <c:crossAx val="1162743616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6829,6 +6831,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7057,11 +7060,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1155157168"/>
-        <c:axId val="1155167664"/>
+        <c:axId val="1158111120"/>
+        <c:axId val="1158113168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1155157168"/>
+        <c:axId val="1158111120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7118,12 +7121,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1155167664"/>
+        <c:crossAx val="1158113168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1155167664"/>
+        <c:axId val="1158113168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7179,7 +7182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1155157168"/>
+        <c:crossAx val="1158111120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13852,15 +13855,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19755</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>70555</xdr:rowOff>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>239889</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>169331</xdr:rowOff>
+      <xdr:rowOff>98777</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -13869,8 +13872,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="330199" y="23184555"/>
-          <a:ext cx="2802468" cy="691443"/>
+          <a:off x="395111" y="23353890"/>
+          <a:ext cx="2737556" cy="451554"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13906,11 +13909,11 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3 outliers</a:t>
+            <a:t>95-97 shortened</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> are the shortened years. Increase was independent of hand check removal, increases again 2013 onwards after a plateau</a:t>
+            <a:t>. Increase not bc of hand check , increases 2013+ after a plateau</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -14071,7 +14074,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> due to shortened 3pt line, 99 and 2012 lower due to lockout. Gradual descent controlling for these from 85 to 04, then jump post rule changes, remains consistent until recent trends.</a:t>
+            <a:t> due to shortened 3pt line, 99 and 2012 lower due to lockout. Gradual ascent to modern era, descent from 85 to 04, then jump post rule changes, not enough evidence for post 2012 trends.</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -14244,7 +14247,7 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.57778</cdr:x>
-      <cdr:y>0.60648</cdr:y>
+      <cdr:y>0.65387</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.94167</cdr:x>
@@ -14257,8 +14260,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2641600" y="1663700"/>
-          <a:ext cx="1663700" cy="749300"/>
+          <a:off x="2701128" y="1742017"/>
+          <a:ext cx="1701190" cy="601474"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -14880,7 +14883,7 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.44988</cdr:x>
-      <cdr:y>0.53151</cdr:y>
+      <cdr:y>0.56329</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.93889</cdr:x>
@@ -14893,8 +14896,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2077156" y="1416050"/>
-          <a:ext cx="2257846" cy="939776"/>
+          <a:off x="2108907" y="1500717"/>
+          <a:ext cx="2292338" cy="855109"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -15042,8 +15045,8 @@
       <cdr:y>0.62037</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.51721</cdr:x>
-      <cdr:y>0.89352</cdr:y>
+      <cdr:x>0.51992</cdr:x>
+      <cdr:y>0.8893</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -15052,8 +15055,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="382514" y="1652774"/>
-          <a:ext cx="1991680" cy="727720"/>
+          <a:off x="389569" y="1652775"/>
+          <a:ext cx="2041069" cy="716479"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -15192,7 +15195,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> as year is a super confounding variable, but I think it makes sense.</a:t>
+            <a:t> as year is a super confounding variable, but I think it makes sense - emphasis shift.</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -15474,8 +15477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15483,25 +15486,28 @@
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="3" max="3" width="5.83203125" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" customWidth="1"/>
-    <col min="8" max="8" width="4" customWidth="1"/>
-    <col min="9" max="11" width="4.83203125" customWidth="1"/>
-    <col min="12" max="13" width="5.83203125" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="8" width="4.33203125" customWidth="1"/>
+    <col min="9" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="11" width="4.83203125" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" customWidth="1"/>
     <col min="14" max="14" width="7.1640625" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="6.83203125" customWidth="1"/>
     <col min="17" max="17" width="7.1640625" customWidth="1"/>
     <col min="18" max="18" width="5.83203125" customWidth="1"/>
     <col min="19" max="20" width="6.83203125" customWidth="1"/>
-    <col min="21" max="23" width="5.83203125" customWidth="1"/>
+    <col min="21" max="21" width="5.83203125" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" customWidth="1"/>
+    <col min="23" max="23" width="6.5" customWidth="1"/>
     <col min="24" max="24" width="6.1640625" customWidth="1"/>
     <col min="25" max="25" width="6.83203125" customWidth="1"/>
     <col min="26" max="28" width="5.83203125" customWidth="1"/>
     <col min="29" max="29" width="7.33203125" customWidth="1"/>
-    <col min="30" max="30" width="6" customWidth="1"/>
+    <col min="30" max="30" width="6.5" customWidth="1"/>
     <col min="31" max="31" width="7.1640625" customWidth="1"/>
     <col min="32" max="32" width="16.6640625" customWidth="1"/>
   </cols>

</xml_diff>